<commit_message>
- patched Excelwriter to actually working status - modified KPI_Zieldatei.xlsx for more comprehendable use
</commit_message>
<xml_diff>
--- a/src/main/resources/KPI_Zieldatei.xlsx
+++ b/src/main/resources/KPI_Zieldatei.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6812322-4813-4F75-97E7-DBC5A6B426C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EE3325-2506-4DC4-A58B-73AD5D707755}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YOY" sheetId="1" r:id="rId1"/>
-    <sheet name="MAXDD" sheetId="3" r:id="rId2"/>
+    <sheet name="MaxDD" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -45,7 +45,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +56,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,7 +109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -112,6 +118,7 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -394,9 +401,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -406,7 +413,7 @@
     <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -424,55 +431,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -486,20 +494,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F768FB-394B-4B4D-A56F-82B8C1EE519B}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD65137-E0AD-42E7-850C-0552F5EEAAE2}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -517,63 +525,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>